<commit_message>
Final Upload - Austin
</commit_message>
<xml_diff>
--- a/data/equity_domestic_5_features.xlsx
+++ b/data/equity_domestic_5_features.xlsx
@@ -2376,7 +2376,7 @@
         <v>-0.01308343832438175</v>
       </c>
       <c r="AU2" t="n">
-        <v>-0.3644929420565463</v>
+        <v>-0.364492942056548</v>
       </c>
       <c r="AV2" t="n">
         <v>1</v>
@@ -2511,13 +2511,13 @@
         <v>14.60287441631134</v>
       </c>
       <c r="CN2" t="n">
-        <v>-17.61625501216349</v>
+        <v>-17.61625501216338</v>
       </c>
       <c r="CO2" t="n">
         <v>0.0040366777845249</v>
       </c>
       <c r="CP2" t="n">
-        <v>-0.3026403020899515</v>
+        <v>-0.3026403020899496</v>
       </c>
       <c r="CQ2" t="n">
         <v>0</v>
@@ -2799,7 +2799,7 @@
         <v>0.008618125787969151</v>
       </c>
       <c r="GF2" t="n">
-        <v>-0.6717247267899209</v>
+        <v>-0.6717247267899206</v>
       </c>
       <c r="GG2" t="n">
         <v>1</v>
@@ -3596,7 +3596,7 @@
         <v>-0.01308343832438175</v>
       </c>
       <c r="CP3" t="n">
-        <v>-0.3644929420565463</v>
+        <v>-0.364492942056548</v>
       </c>
       <c r="CQ3" t="n">
         <v>1</v>
@@ -3731,13 +3731,13 @@
         <v>14.60287441631134</v>
       </c>
       <c r="EI3" t="n">
-        <v>-17.61625501216349</v>
+        <v>-17.61625501216338</v>
       </c>
       <c r="EJ3" t="n">
         <v>0.0040366777845249</v>
       </c>
       <c r="EK3" t="n">
-        <v>-0.3026403020899515</v>
+        <v>-0.3026403020899496</v>
       </c>
       <c r="EL3" t="n">
         <v>0</v>
@@ -3872,13 +3872,13 @@
         <v>31.61706504881646</v>
       </c>
       <c r="GD3" t="n">
-        <v>161.4005369077002</v>
+        <v>161.4005369076999</v>
       </c>
       <c r="GE3" t="n">
         <v>0.02579551559991698</v>
       </c>
       <c r="GF3" t="n">
-        <v>0.318950427929075</v>
+        <v>0.3189504279290792</v>
       </c>
       <c r="GG3" t="n">
         <v>1</v>
@@ -4154,13 +4154,13 @@
         <v>19.67790539125385</v>
       </c>
       <c r="JT3" t="n">
-        <v>27.88394380625192</v>
+        <v>27.88394380625194</v>
       </c>
       <c r="JU3" t="n">
         <v>-0.000231949507706735</v>
       </c>
       <c r="JV3" t="n">
-        <v>0.4676821352021773</v>
+        <v>0.4676821352021775</v>
       </c>
       <c r="JW3" t="n">
         <v>0</v>
@@ -4816,7 +4816,7 @@
         <v>-0.01308343832438175</v>
       </c>
       <c r="EK4" t="n">
-        <v>-0.3644929420565463</v>
+        <v>-0.364492942056548</v>
       </c>
       <c r="EL4" t="n">
         <v>1</v>
@@ -5098,7 +5098,7 @@
         <v>0.008618125787969151</v>
       </c>
       <c r="IA4" t="n">
-        <v>-0.6717247267899209</v>
+        <v>-0.6717247267899206</v>
       </c>
       <c r="IB4" t="n">
         <v>1</v>
@@ -5233,13 +5233,13 @@
         <v>20.47124843687621</v>
       </c>
       <c r="JT4" t="n">
-        <v>196.4776686435681</v>
+        <v>196.4776686435679</v>
       </c>
       <c r="JU4" t="n">
         <v>0.00683333051226351</v>
       </c>
       <c r="JV4" t="n">
-        <v>-0.2836416176878022</v>
+        <v>-0.2836416176877976</v>
       </c>
       <c r="JW4" t="n">
         <v>1</v>
@@ -6030,13 +6030,13 @@
         <v>14.60287441631134</v>
       </c>
       <c r="GD5" t="n">
-        <v>-17.61625501216349</v>
+        <v>-17.61625501216338</v>
       </c>
       <c r="GE5" t="n">
         <v>0.0040366777845249</v>
       </c>
       <c r="GF5" t="n">
-        <v>-0.3026403020899515</v>
+        <v>-0.3026403020899496</v>
       </c>
       <c r="GG5" t="n">
         <v>0</v>
@@ -6171,13 +6171,13 @@
         <v>31.61706504881646</v>
       </c>
       <c r="HY5" t="n">
-        <v>161.4005369077002</v>
+        <v>161.4005369076999</v>
       </c>
       <c r="HZ5" t="n">
         <v>0.02579551559991698</v>
       </c>
       <c r="IA5" t="n">
-        <v>0.318950427929075</v>
+        <v>0.3189504279290792</v>
       </c>
       <c r="IB5" t="n">
         <v>1</v>
@@ -6312,13 +6312,13 @@
         <v>15.31085069395273</v>
       </c>
       <c r="JT5" t="n">
-        <v>-24.17347568496916</v>
+        <v>-24.17347568496911</v>
       </c>
       <c r="JU5" t="n">
         <v>-0.0124880311843039</v>
       </c>
       <c r="JV5" t="n">
-        <v>-0.4095007361193496</v>
+        <v>-0.4095007361193487</v>
       </c>
       <c r="JW5" t="n">
         <v>0</v>
@@ -6692,7 +6692,7 @@
         <v>-0.009379054016029538</v>
       </c>
       <c r="AU6" t="n">
-        <v>-0.8511962813175912</v>
+        <v>-0.8511962813175913</v>
       </c>
       <c r="AV6" t="n">
         <v>0</v>
@@ -7115,7 +7115,7 @@
         <v>-0.01308343832438175</v>
       </c>
       <c r="GF6" t="n">
-        <v>-0.3644929420565463</v>
+        <v>-0.364492942056548</v>
       </c>
       <c r="GG6" t="n">
         <v>1</v>
@@ -7391,13 +7391,13 @@
         <v>18.3555362383239</v>
       </c>
       <c r="JT6" t="n">
-        <v>132.6627880711566</v>
+        <v>132.6627880711565</v>
       </c>
       <c r="JU6" t="n">
         <v>0.01668558144701267</v>
       </c>
       <c r="JV6" t="n">
-        <v>0.7353548849425307</v>
+        <v>0.7353548849425317</v>
       </c>
       <c r="JW6" t="n">
         <v>0</v>
@@ -7765,13 +7765,13 @@
         <v>23.33125174904285</v>
       </c>
       <c r="AS7" t="n">
-        <v>62.61106509398657</v>
+        <v>62.61106509398633</v>
       </c>
       <c r="AT7" t="n">
         <v>-0.04055884011203448</v>
       </c>
       <c r="AU7" t="n">
-        <v>0.8879042434308362</v>
+        <v>0.8879042434308342</v>
       </c>
       <c r="AV7" t="n">
         <v>1</v>
@@ -7912,7 +7912,7 @@
         <v>-0.009379054016029538</v>
       </c>
       <c r="CP7" t="n">
-        <v>-0.8511962813175912</v>
+        <v>-0.8511962813175913</v>
       </c>
       <c r="CQ7" t="n">
         <v>0</v>
@@ -8329,13 +8329,13 @@
         <v>14.60287441631134</v>
       </c>
       <c r="HY7" t="n">
-        <v>-17.61625501216349</v>
+        <v>-17.61625501216338</v>
       </c>
       <c r="HZ7" t="n">
         <v>0.0040366777845249</v>
       </c>
       <c r="IA7" t="n">
-        <v>-0.3026403020899515</v>
+        <v>-0.3026403020899496</v>
       </c>
       <c r="IB7" t="n">
         <v>0</v>
@@ -8476,7 +8476,7 @@
         <v>-0.009185480811320739</v>
       </c>
       <c r="JV7" t="n">
-        <v>-0.5479717827526265</v>
+        <v>-0.5479717827526266</v>
       </c>
       <c r="JW7" t="n">
         <v>1</v>
@@ -8985,13 +8985,13 @@
         <v>23.33125174904285</v>
       </c>
       <c r="CN8" t="n">
-        <v>62.61106509398657</v>
+        <v>62.61106509398633</v>
       </c>
       <c r="CO8" t="n">
         <v>-0.04055884011203448</v>
       </c>
       <c r="CP8" t="n">
-        <v>0.8879042434308362</v>
+        <v>0.8879042434308342</v>
       </c>
       <c r="CQ8" t="n">
         <v>1</v>
@@ -9132,7 +9132,7 @@
         <v>-0.009379054016029538</v>
       </c>
       <c r="EK8" t="n">
-        <v>-0.8511962813175912</v>
+        <v>-0.8511962813175913</v>
       </c>
       <c r="EL8" t="n">
         <v>0</v>
@@ -9414,7 +9414,7 @@
         <v>-0.01308343832438175</v>
       </c>
       <c r="IA8" t="n">
-        <v>-0.3644929420565463</v>
+        <v>-0.364492942056548</v>
       </c>
       <c r="IB8" t="n">
         <v>1</v>
@@ -10205,13 +10205,13 @@
         <v>23.33125174904285</v>
       </c>
       <c r="EI9" t="n">
-        <v>62.61106509398657</v>
+        <v>62.61106509398633</v>
       </c>
       <c r="EJ9" t="n">
         <v>-0.04055884011203448</v>
       </c>
       <c r="EK9" t="n">
-        <v>0.8879042434308362</v>
+        <v>0.8879042434308342</v>
       </c>
       <c r="EL9" t="n">
         <v>1</v>
@@ -11431,7 +11431,7 @@
         <v>-0.009379054016029538</v>
       </c>
       <c r="GF10" t="n">
-        <v>-0.8511962813175912</v>
+        <v>-0.8511962813175913</v>
       </c>
       <c r="GG10" t="n">
         <v>0</v>
@@ -11713,7 +11713,7 @@
         <v>0.008618125787969151</v>
       </c>
       <c r="JV10" t="n">
-        <v>-0.6717247267899209</v>
+        <v>-0.6717247267899206</v>
       </c>
       <c r="JW10" t="n">
         <v>1</v>
@@ -12504,13 +12504,13 @@
         <v>23.33125174904285</v>
       </c>
       <c r="GD11" t="n">
-        <v>62.61106509398657</v>
+        <v>62.61106509398633</v>
       </c>
       <c r="GE11" t="n">
         <v>-0.04055884011203448</v>
       </c>
       <c r="GF11" t="n">
-        <v>0.8879042434308362</v>
+        <v>0.8879042434308342</v>
       </c>
       <c r="GG11" t="n">
         <v>1</v>
@@ -12786,13 +12786,13 @@
         <v>31.61706504881646</v>
       </c>
       <c r="JT11" t="n">
-        <v>161.4005369077002</v>
+        <v>161.4005369076999</v>
       </c>
       <c r="JU11" t="n">
         <v>0.02579551559991698</v>
       </c>
       <c r="JV11" t="n">
-        <v>0.318950427929075</v>
+        <v>0.3189504279290792</v>
       </c>
       <c r="JW11" t="n">
         <v>1</v>
@@ -13730,7 +13730,7 @@
         <v>-0.009379054016029538</v>
       </c>
       <c r="IA12" t="n">
-        <v>-0.8511962813175912</v>
+        <v>-0.8511962813175913</v>
       </c>
       <c r="IB12" t="n">
         <v>0</v>
@@ -14803,13 +14803,13 @@
         <v>23.33125174904285</v>
       </c>
       <c r="HY13" t="n">
-        <v>62.61106509398657</v>
+        <v>62.61106509398633</v>
       </c>
       <c r="HZ13" t="n">
         <v>-0.04055884011203448</v>
       </c>
       <c r="IA13" t="n">
-        <v>0.8879042434308362</v>
+        <v>0.8879042434308342</v>
       </c>
       <c r="IB13" t="n">
         <v>1</v>
@@ -14944,13 +14944,13 @@
         <v>14.60287441631134</v>
       </c>
       <c r="JT13" t="n">
-        <v>-17.61625501216349</v>
+        <v>-17.61625501216338</v>
       </c>
       <c r="JU13" t="n">
         <v>0.0040366777845249</v>
       </c>
       <c r="JV13" t="n">
-        <v>-0.3026403020899515</v>
+        <v>-0.3026403020899496</v>
       </c>
       <c r="JW13" t="n">
         <v>0</v>
@@ -16029,7 +16029,7 @@
         <v>-0.01308343832438175</v>
       </c>
       <c r="JV14" t="n">
-        <v>-0.3644929420565463</v>
+        <v>-0.364492942056548</v>
       </c>
       <c r="JW14" t="n">
         <v>1</v>
@@ -16397,7 +16397,7 @@
         <v>17.34380404863938</v>
       </c>
       <c r="AS15" t="n">
-        <v>89.4805857248502</v>
+        <v>89.48058572485029</v>
       </c>
       <c r="AT15" t="n">
         <v>-0.002200376720612546</v>
@@ -17617,7 +17617,7 @@
         <v>17.34380404863938</v>
       </c>
       <c r="CN16" t="n">
-        <v>89.4805857248502</v>
+        <v>89.48058572485029</v>
       </c>
       <c r="CO16" t="n">
         <v>-0.002200376720612546</v>
@@ -18837,7 +18837,7 @@
         <v>17.34380404863938</v>
       </c>
       <c r="EI17" t="n">
-        <v>89.4805857248502</v>
+        <v>89.48058572485029</v>
       </c>
       <c r="EJ17" t="n">
         <v>-0.002200376720612546</v>
@@ -20345,7 +20345,7 @@
         <v>-0.009379054016029538</v>
       </c>
       <c r="JV18" t="n">
-        <v>-0.8511962813175912</v>
+        <v>-0.8511962813175913</v>
       </c>
       <c r="JW18" t="n">
         <v>0</v>
@@ -21136,7 +21136,7 @@
         <v>17.34380404863938</v>
       </c>
       <c r="GD19" t="n">
-        <v>89.4805857248502</v>
+        <v>89.48058572485029</v>
       </c>
       <c r="GE19" t="n">
         <v>-0.002200376720612546</v>
@@ -21418,13 +21418,13 @@
         <v>23.33125174904285</v>
       </c>
       <c r="JT19" t="n">
-        <v>62.61106509398657</v>
+        <v>62.61106509398633</v>
       </c>
       <c r="JU19" t="n">
         <v>-0.04055884011203448</v>
       </c>
       <c r="JV19" t="n">
-        <v>0.8879042434308362</v>
+        <v>0.8879042434308342</v>
       </c>
       <c r="JW19" t="n">
         <v>1</v>
@@ -21792,13 +21792,13 @@
         <v>22.25295516419822</v>
       </c>
       <c r="AS20" t="n">
-        <v>206.9440377836906</v>
+        <v>206.9440377836897</v>
       </c>
       <c r="AT20" t="n">
         <v>0.0002355551976266059</v>
       </c>
       <c r="AU20" t="n">
-        <v>-0.4531200150402392</v>
+        <v>-0.4531200150402242</v>
       </c>
       <c r="AV20" t="n">
         <v>0</v>
@@ -23012,13 +23012,13 @@
         <v>22.25295516419822</v>
       </c>
       <c r="CN21" t="n">
-        <v>206.9440377836906</v>
+        <v>206.9440377836897</v>
       </c>
       <c r="CO21" t="n">
         <v>0.0002355551976266059</v>
       </c>
       <c r="CP21" t="n">
-        <v>-0.4531200150402392</v>
+        <v>-0.4531200150402242</v>
       </c>
       <c r="CQ21" t="n">
         <v>0</v>
@@ -23435,7 +23435,7 @@
         <v>17.34380404863938</v>
       </c>
       <c r="HY21" t="n">
-        <v>89.4805857248502</v>
+        <v>89.48058572485029</v>
       </c>
       <c r="HZ21" t="n">
         <v>-0.002200376720612546</v>
@@ -24232,13 +24232,13 @@
         <v>22.25295516419822</v>
       </c>
       <c r="EI22" t="n">
-        <v>206.9440377836906</v>
+        <v>206.9440377836897</v>
       </c>
       <c r="EJ22" t="n">
         <v>0.0002355551976266059</v>
       </c>
       <c r="EK22" t="n">
-        <v>-0.4531200150402392</v>
+        <v>-0.4531200150402242</v>
       </c>
       <c r="EL22" t="n">
         <v>0</v>
@@ -25035,7 +25035,7 @@
         <v>0.01001018396944395</v>
       </c>
       <c r="AU23" t="n">
-        <v>-0.6205862823993451</v>
+        <v>-0.6205862823993448</v>
       </c>
       <c r="AV23" t="n">
         <v>1</v>
@@ -26255,7 +26255,7 @@
         <v>0.01001018396944395</v>
       </c>
       <c r="CP24" t="n">
-        <v>-0.6205862823993451</v>
+        <v>-0.6205862823993448</v>
       </c>
       <c r="CQ24" t="n">
         <v>1</v>
@@ -26531,13 +26531,13 @@
         <v>22.25295516419822</v>
       </c>
       <c r="GD24" t="n">
-        <v>206.9440377836906</v>
+        <v>206.9440377836897</v>
       </c>
       <c r="GE24" t="n">
         <v>0.0002355551976266059</v>
       </c>
       <c r="GF24" t="n">
-        <v>-0.4531200150402392</v>
+        <v>-0.4531200150402242</v>
       </c>
       <c r="GG24" t="n">
         <v>0</v>
@@ -27187,13 +27187,13 @@
         <v>20.57293259710981</v>
       </c>
       <c r="AS25" t="n">
-        <v>163.7885303755892</v>
+        <v>163.788530375589</v>
       </c>
       <c r="AT25" t="n">
         <v>0.01694451092157209</v>
       </c>
       <c r="AU25" t="n">
-        <v>0.2791833346402564</v>
+        <v>0.2791833346402602</v>
       </c>
       <c r="AV25" t="n">
         <v>1</v>
@@ -27475,7 +27475,7 @@
         <v>0.01001018396944395</v>
       </c>
       <c r="EK25" t="n">
-        <v>-0.6205862823993451</v>
+        <v>-0.6205862823993448</v>
       </c>
       <c r="EL25" t="n">
         <v>1</v>
@@ -28407,13 +28407,13 @@
         <v>20.57293259710981</v>
       </c>
       <c r="CN26" t="n">
-        <v>163.7885303755892</v>
+        <v>163.788530375589</v>
       </c>
       <c r="CO26" t="n">
         <v>0.01694451092157209</v>
       </c>
       <c r="CP26" t="n">
-        <v>0.2791833346402564</v>
+        <v>0.2791833346402602</v>
       </c>
       <c r="CQ26" t="n">
         <v>1</v>
@@ -28830,13 +28830,13 @@
         <v>22.25295516419822</v>
       </c>
       <c r="HY26" t="n">
-        <v>206.9440377836906</v>
+        <v>206.9440377836897</v>
       </c>
       <c r="HZ26" t="n">
         <v>0.0002355551976266059</v>
       </c>
       <c r="IA26" t="n">
-        <v>-0.4531200150402392</v>
+        <v>-0.4531200150402242</v>
       </c>
       <c r="IB26" t="n">
         <v>0</v>
@@ -29627,13 +29627,13 @@
         <v>20.57293259710981</v>
       </c>
       <c r="EI27" t="n">
-        <v>163.7885303755892</v>
+        <v>163.788530375589</v>
       </c>
       <c r="EJ27" t="n">
         <v>0.01694451092157209</v>
       </c>
       <c r="EK27" t="n">
-        <v>0.2791833346402564</v>
+        <v>0.2791833346402602</v>
       </c>
       <c r="EL27" t="n">
         <v>1</v>
@@ -29774,7 +29774,7 @@
         <v>0.01001018396944395</v>
       </c>
       <c r="GF27" t="n">
-        <v>-0.6205862823993451</v>
+        <v>-0.6205862823993448</v>
       </c>
       <c r="GG27" t="n">
         <v>1</v>
@@ -30050,7 +30050,7 @@
         <v>17.34380404863938</v>
       </c>
       <c r="JT27" t="n">
-        <v>89.4805857248502</v>
+        <v>89.48058572485029</v>
       </c>
       <c r="JU27" t="n">
         <v>-0.002200376720612546</v>
@@ -31926,13 +31926,13 @@
         <v>20.57293259710981</v>
       </c>
       <c r="GD29" t="n">
-        <v>163.7885303755892</v>
+        <v>163.788530375589</v>
       </c>
       <c r="GE29" t="n">
         <v>0.01694451092157209</v>
       </c>
       <c r="GF29" t="n">
-        <v>0.2791833346402564</v>
+        <v>0.2791833346402602</v>
       </c>
       <c r="GG29" t="n">
         <v>1</v>
@@ -32073,7 +32073,7 @@
         <v>0.01001018396944395</v>
       </c>
       <c r="IA29" t="n">
-        <v>-0.6205862823993451</v>
+        <v>-0.6205862823993448</v>
       </c>
       <c r="IB29" t="n">
         <v>1</v>
@@ -34225,13 +34225,13 @@
         <v>20.57293259710981</v>
       </c>
       <c r="HY31" t="n">
-        <v>163.7885303755892</v>
+        <v>163.788530375589</v>
       </c>
       <c r="HZ31" t="n">
         <v>0.01694451092157209</v>
       </c>
       <c r="IA31" t="n">
-        <v>0.2791833346402564</v>
+        <v>0.2791833346402602</v>
       </c>
       <c r="IB31" t="n">
         <v>1</v>
@@ -34746,7 +34746,7 @@
         <v>0.0487291059314266</v>
       </c>
       <c r="AU32" t="n">
-        <v>0.3967258022628586</v>
+        <v>0.3967258022628585</v>
       </c>
       <c r="AV32" t="n">
         <v>1</v>
@@ -35445,13 +35445,13 @@
         <v>22.25295516419822</v>
       </c>
       <c r="JT32" t="n">
-        <v>206.9440377836906</v>
+        <v>206.9440377836897</v>
       </c>
       <c r="JU32" t="n">
         <v>0.0002355551976266059</v>
       </c>
       <c r="JV32" t="n">
-        <v>-0.4531200150402392</v>
+        <v>-0.4531200150402242</v>
       </c>
       <c r="JW32" t="n">
         <v>0</v>
@@ -35966,7 +35966,7 @@
         <v>0.0487291059314266</v>
       </c>
       <c r="CP33" t="n">
-        <v>0.3967258022628586</v>
+        <v>0.3967258022628585</v>
       </c>
       <c r="CQ33" t="n">
         <v>1</v>
@@ -36898,13 +36898,13 @@
         <v>17.22464100555703</v>
       </c>
       <c r="AS34" t="n">
-        <v>30.71676638348169</v>
+        <v>30.71676638348174</v>
       </c>
       <c r="AT34" t="n">
         <v>-0.01917503053980575</v>
       </c>
       <c r="AU34" t="n">
-        <v>0.5107945134112335</v>
+        <v>0.5107945134112344</v>
       </c>
       <c r="AV34" t="n">
         <v>1</v>
@@ -37186,7 +37186,7 @@
         <v>0.0487291059314266</v>
       </c>
       <c r="EK34" t="n">
-        <v>0.3967258022628586</v>
+        <v>0.3967258022628585</v>
       </c>
       <c r="EL34" t="n">
         <v>1</v>
@@ -38118,13 +38118,13 @@
         <v>17.22464100555703</v>
       </c>
       <c r="CN35" t="n">
-        <v>30.71676638348169</v>
+        <v>30.71676638348174</v>
       </c>
       <c r="CO35" t="n">
         <v>-0.01917503053980575</v>
       </c>
       <c r="CP35" t="n">
-        <v>0.5107945134112335</v>
+        <v>0.5107945134112344</v>
       </c>
       <c r="CQ35" t="n">
         <v>1</v>
@@ -38688,7 +38688,7 @@
         <v>0.01001018396944395</v>
       </c>
       <c r="JV35" t="n">
-        <v>-0.6205862823993451</v>
+        <v>-0.6205862823993448</v>
       </c>
       <c r="JW35" t="n">
         <v>1</v>
@@ -39056,13 +39056,13 @@
         <v>24.88372282164005</v>
       </c>
       <c r="AS36" t="n">
-        <v>278.4905559137335</v>
+        <v>278.4905559137336</v>
       </c>
       <c r="AT36" t="n">
         <v>-0.05894374067556868</v>
       </c>
       <c r="AU36" t="n">
-        <v>-0.9890402134108792</v>
+        <v>-0.9890402134108789</v>
       </c>
       <c r="AV36" t="n">
         <v>1</v>
@@ -39338,13 +39338,13 @@
         <v>17.22464100555703</v>
       </c>
       <c r="EI36" t="n">
-        <v>30.71676638348169</v>
+        <v>30.71676638348174</v>
       </c>
       <c r="EJ36" t="n">
         <v>-0.01917503053980575</v>
       </c>
       <c r="EK36" t="n">
-        <v>0.5107945134112335</v>
+        <v>0.5107945134112344</v>
       </c>
       <c r="EL36" t="n">
         <v>1</v>
@@ -39485,7 +39485,7 @@
         <v>0.0487291059314266</v>
       </c>
       <c r="GF36" t="n">
-        <v>0.3967258022628586</v>
+        <v>0.3967258022628585</v>
       </c>
       <c r="GG36" t="n">
         <v>1</v>
@@ -40276,13 +40276,13 @@
         <v>24.88372282164005</v>
       </c>
       <c r="CN37" t="n">
-        <v>278.4905559137335</v>
+        <v>278.4905559137336</v>
       </c>
       <c r="CO37" t="n">
         <v>-0.05894374067556868</v>
       </c>
       <c r="CP37" t="n">
-        <v>-0.9890402134108792</v>
+        <v>-0.9890402134108789</v>
       </c>
       <c r="CQ37" t="n">
         <v>1</v>
@@ -40840,13 +40840,13 @@
         <v>20.57293259710981</v>
       </c>
       <c r="JT37" t="n">
-        <v>163.7885303755892</v>
+        <v>163.788530375589</v>
       </c>
       <c r="JU37" t="n">
         <v>0.01694451092157209</v>
       </c>
       <c r="JV37" t="n">
-        <v>0.2791833346402564</v>
+        <v>0.2791833346402602</v>
       </c>
       <c r="JW37" t="n">
         <v>1</v>
@@ -41496,13 +41496,13 @@
         <v>24.88372282164005</v>
       </c>
       <c r="EI38" t="n">
-        <v>278.4905559137335</v>
+        <v>278.4905559137336</v>
       </c>
       <c r="EJ38" t="n">
         <v>-0.05894374067556868</v>
       </c>
       <c r="EK38" t="n">
-        <v>-0.9890402134108792</v>
+        <v>-0.9890402134108789</v>
       </c>
       <c r="EL38" t="n">
         <v>1</v>
@@ -41637,13 +41637,13 @@
         <v>17.22464100555703</v>
       </c>
       <c r="GD38" t="n">
-        <v>30.71676638348169</v>
+        <v>30.71676638348174</v>
       </c>
       <c r="GE38" t="n">
         <v>-0.01917503053980575</v>
       </c>
       <c r="GF38" t="n">
-        <v>0.5107945134112335</v>
+        <v>0.5107945134112344</v>
       </c>
       <c r="GG38" t="n">
         <v>1</v>
@@ -41784,7 +41784,7 @@
         <v>0.0487291059314266</v>
       </c>
       <c r="IA38" t="n">
-        <v>0.3967258022628586</v>
+        <v>0.3967258022628585</v>
       </c>
       <c r="IB38" t="n">
         <v>1</v>
@@ -42293,13 +42293,13 @@
         <v>19.32285611649471</v>
       </c>
       <c r="AS39" t="n">
-        <v>163.5600796632013</v>
+        <v>163.5600796632012</v>
       </c>
       <c r="AT39" t="n">
         <v>0.02885339639708224</v>
       </c>
       <c r="AU39" t="n">
-        <v>0.2830097819384235</v>
+        <v>0.2830097819384243</v>
       </c>
       <c r="AV39" t="n">
         <v>1</v>
@@ -43513,13 +43513,13 @@
         <v>19.32285611649471</v>
       </c>
       <c r="CN40" t="n">
-        <v>163.5600796632013</v>
+        <v>163.5600796632012</v>
       </c>
       <c r="CO40" t="n">
         <v>0.02885339639708224</v>
       </c>
       <c r="CP40" t="n">
-        <v>0.2830097819384235</v>
+        <v>0.2830097819384243</v>
       </c>
       <c r="CQ40" t="n">
         <v>1</v>
@@ -43795,13 +43795,13 @@
         <v>24.88372282164005</v>
       </c>
       <c r="GD40" t="n">
-        <v>278.4905559137335</v>
+        <v>278.4905559137336</v>
       </c>
       <c r="GE40" t="n">
         <v>-0.05894374067556868</v>
       </c>
       <c r="GF40" t="n">
-        <v>-0.9890402134108792</v>
+        <v>-0.9890402134108789</v>
       </c>
       <c r="GG40" t="n">
         <v>1</v>
@@ -43936,13 +43936,13 @@
         <v>17.22464100555703</v>
       </c>
       <c r="HY40" t="n">
-        <v>30.71676638348169</v>
+        <v>30.71676638348174</v>
       </c>
       <c r="HZ40" t="n">
         <v>-0.01917503053980575</v>
       </c>
       <c r="IA40" t="n">
-        <v>0.5107945134112335</v>
+        <v>0.5107945134112344</v>
       </c>
       <c r="IB40" t="n">
         <v>1</v>
@@ -44733,13 +44733,13 @@
         <v>19.32285611649471</v>
       </c>
       <c r="EI41" t="n">
-        <v>163.5600796632013</v>
+        <v>163.5600796632012</v>
       </c>
       <c r="EJ41" t="n">
         <v>0.02885339639708224</v>
       </c>
       <c r="EK41" t="n">
-        <v>0.2830097819384235</v>
+        <v>0.2830097819384243</v>
       </c>
       <c r="EL41" t="n">
         <v>1</v>
@@ -46094,13 +46094,13 @@
         <v>24.88372282164005</v>
       </c>
       <c r="HY42" t="n">
-        <v>278.4905559137335</v>
+        <v>278.4905559137336</v>
       </c>
       <c r="HZ42" t="n">
         <v>-0.05894374067556868</v>
       </c>
       <c r="IA42" t="n">
-        <v>-0.9890402134108792</v>
+        <v>-0.9890402134108789</v>
       </c>
       <c r="IB42" t="n">
         <v>1</v>
@@ -47032,13 +47032,13 @@
         <v>19.32285611649471</v>
       </c>
       <c r="GD43" t="n">
-        <v>163.5600796632013</v>
+        <v>163.5600796632012</v>
       </c>
       <c r="GE43" t="n">
         <v>0.02885339639708224</v>
       </c>
       <c r="GF43" t="n">
-        <v>0.2830097819384235</v>
+        <v>0.2830097819384243</v>
       </c>
       <c r="GG43" t="n">
         <v>1</v>
@@ -47688,13 +47688,13 @@
         <v>35.17717231077314</v>
       </c>
       <c r="AS44" t="n">
-        <v>-13.22557956059632</v>
+        <v>-13.22557956059597</v>
       </c>
       <c r="AT44" t="n">
         <v>0.008874889197968361</v>
       </c>
       <c r="AU44" t="n">
-        <v>-0.2287854992587356</v>
+        <v>-0.2287854992587298</v>
       </c>
       <c r="AV44" t="n">
         <v>0</v>
@@ -48399,7 +48399,7 @@
         <v>0.0487291059314266</v>
       </c>
       <c r="JV44" t="n">
-        <v>0.3967258022628586</v>
+        <v>0.3967258022628585</v>
       </c>
       <c r="JW44" t="n">
         <v>1</v>
@@ -48908,13 +48908,13 @@
         <v>35.17717231077314</v>
       </c>
       <c r="CN45" t="n">
-        <v>-13.22557956059632</v>
+        <v>-13.22557956059597</v>
       </c>
       <c r="CO45" t="n">
         <v>0.008874889197968361</v>
       </c>
       <c r="CP45" t="n">
-        <v>-0.2287854992587356</v>
+        <v>-0.2287854992587298</v>
       </c>
       <c r="CQ45" t="n">
         <v>0</v>
@@ -49331,13 +49331,13 @@
         <v>19.32285611649471</v>
       </c>
       <c r="HY45" t="n">
-        <v>163.5600796632013</v>
+        <v>163.5600796632012</v>
       </c>
       <c r="HZ45" t="n">
         <v>0.02885339639708224</v>
       </c>
       <c r="IA45" t="n">
-        <v>0.2830097819384235</v>
+        <v>0.2830097819384243</v>
       </c>
       <c r="IB45" t="n">
         <v>1</v>
@@ -50128,13 +50128,13 @@
         <v>35.17717231077314</v>
       </c>
       <c r="EI46" t="n">
-        <v>-13.22557956059632</v>
+        <v>-13.22557956059597</v>
       </c>
       <c r="EJ46" t="n">
         <v>0.008874889197968361</v>
       </c>
       <c r="EK46" t="n">
-        <v>-0.2287854992587356</v>
+        <v>-0.2287854992587298</v>
       </c>
       <c r="EL46" t="n">
         <v>0</v>
@@ -50551,13 +50551,13 @@
         <v>17.22464100555703</v>
       </c>
       <c r="JT46" t="n">
-        <v>30.71676638348169</v>
+        <v>30.71676638348174</v>
       </c>
       <c r="JU46" t="n">
         <v>-0.01917503053980575</v>
       </c>
       <c r="JV46" t="n">
-        <v>0.5107945134112335</v>
+        <v>0.5107945134112344</v>
       </c>
       <c r="JW46" t="n">
         <v>1</v>
@@ -52004,13 +52004,13 @@
         <v>17.817149360139</v>
       </c>
       <c r="AS48" t="n">
-        <v>195.8843408692714</v>
+        <v>195.8843408692713</v>
       </c>
       <c r="AT48" t="n">
         <v>-0.004492534230547332</v>
       </c>
       <c r="AU48" t="n">
-        <v>-0.273696361304601</v>
+        <v>-0.2736963613045997</v>
       </c>
       <c r="AV48" t="n">
         <v>1</v>
@@ -52427,13 +52427,13 @@
         <v>35.17717231077314</v>
       </c>
       <c r="GD48" t="n">
-        <v>-13.22557956059632</v>
+        <v>-13.22557956059597</v>
       </c>
       <c r="GE48" t="n">
         <v>0.008874889197968361</v>
       </c>
       <c r="GF48" t="n">
-        <v>-0.2287854992587356</v>
+        <v>-0.2287854992587298</v>
       </c>
       <c r="GG48" t="n">
         <v>0</v>
@@ -52709,13 +52709,13 @@
         <v>24.88372282164005</v>
       </c>
       <c r="JT48" t="n">
-        <v>278.4905559137335</v>
+        <v>278.4905559137336</v>
       </c>
       <c r="JU48" t="n">
         <v>-0.05894374067556868</v>
       </c>
       <c r="JV48" t="n">
-        <v>-0.9890402134108792</v>
+        <v>-0.9890402134108789</v>
       </c>
       <c r="JW48" t="n">
         <v>1</v>
@@ -53083,13 +53083,13 @@
         <v>22.04708776193247</v>
       </c>
       <c r="AS49" t="n">
-        <v>-25.12804529840878</v>
+        <v>-25.12804529840957</v>
       </c>
       <c r="AT49" t="n">
         <v>-0.03156768979392504</v>
       </c>
       <c r="AU49" t="n">
-        <v>-0.4246426322585574</v>
+        <v>-0.4246426322585699</v>
       </c>
       <c r="AV49" t="n">
         <v>0</v>
@@ -53224,13 +53224,13 @@
         <v>17.817149360139</v>
       </c>
       <c r="CN49" t="n">
-        <v>195.8843408692714</v>
+        <v>195.8843408692713</v>
       </c>
       <c r="CO49" t="n">
         <v>-0.004492534230547332</v>
       </c>
       <c r="CP49" t="n">
-        <v>-0.273696361304601</v>
+        <v>-0.2736963613045997</v>
       </c>
       <c r="CQ49" t="n">
         <v>1</v>
@@ -54303,13 +54303,13 @@
         <v>22.04708776193247</v>
       </c>
       <c r="CN50" t="n">
-        <v>-25.12804529840878</v>
+        <v>-25.12804529840957</v>
       </c>
       <c r="CO50" t="n">
         <v>-0.03156768979392504</v>
       </c>
       <c r="CP50" t="n">
-        <v>-0.4246426322585574</v>
+        <v>-0.4246426322585699</v>
       </c>
       <c r="CQ50" t="n">
         <v>0</v>
@@ -54444,13 +54444,13 @@
         <v>17.817149360139</v>
       </c>
       <c r="EI50" t="n">
-        <v>195.8843408692714</v>
+        <v>195.8843408692713</v>
       </c>
       <c r="EJ50" t="n">
         <v>-0.004492534230547332</v>
       </c>
       <c r="EK50" t="n">
-        <v>-0.273696361304601</v>
+        <v>-0.2736963613045997</v>
       </c>
       <c r="EL50" t="n">
         <v>1</v>
@@ -54726,13 +54726,13 @@
         <v>35.17717231077314</v>
       </c>
       <c r="HY50" t="n">
-        <v>-13.22557956059632</v>
+        <v>-13.22557956059597</v>
       </c>
       <c r="HZ50" t="n">
         <v>0.008874889197968361</v>
       </c>
       <c r="IA50" t="n">
-        <v>-0.2287854992587356</v>
+        <v>-0.2287854992587298</v>
       </c>
       <c r="IB50" t="n">
         <v>0</v>
@@ -55241,13 +55241,13 @@
         <v>22.58902988139615</v>
       </c>
       <c r="AS51" t="n">
-        <v>211.950518950205</v>
+        <v>211.9505189502051</v>
       </c>
       <c r="AT51" t="n">
         <v>0.005792212006757475</v>
       </c>
       <c r="AU51" t="n">
-        <v>-0.529186686240193</v>
+        <v>-0.5291866862401938</v>
       </c>
       <c r="AV51" t="n">
         <v>1</v>
@@ -55523,13 +55523,13 @@
         <v>22.04708776193247</v>
       </c>
       <c r="EI51" t="n">
-        <v>-25.12804529840878</v>
+        <v>-25.12804529840957</v>
       </c>
       <c r="EJ51" t="n">
         <v>-0.03156768979392504</v>
       </c>
       <c r="EK51" t="n">
-        <v>-0.4246426322585574</v>
+        <v>-0.4246426322585699</v>
       </c>
       <c r="EL51" t="n">
         <v>0</v>
@@ -55946,13 +55946,13 @@
         <v>19.32285611649471</v>
       </c>
       <c r="JT51" t="n">
-        <v>163.5600796632013</v>
+        <v>163.5600796632012</v>
       </c>
       <c r="JU51" t="n">
         <v>0.02885339639708224</v>
       </c>
       <c r="JV51" t="n">
-        <v>0.2830097819384235</v>
+        <v>0.2830097819384243</v>
       </c>
       <c r="JW51" t="n">
         <v>1</v>
@@ -56320,13 +56320,13 @@
         <v>19.24209327631613</v>
       </c>
       <c r="AS52" t="n">
-        <v>88.19775683135879</v>
+        <v>88.19775683135845</v>
       </c>
       <c r="AT52" t="n">
         <v>0.02773085948231207</v>
       </c>
       <c r="AU52" t="n">
-        <v>0.9995053298471932</v>
+        <v>0.999505329847193</v>
       </c>
       <c r="AV52" t="n">
         <v>0</v>
@@ -56461,13 +56461,13 @@
         <v>22.58902988139615</v>
       </c>
       <c r="CN52" t="n">
-        <v>211.950518950205</v>
+        <v>211.9505189502051</v>
       </c>
       <c r="CO52" t="n">
         <v>0.005792212006757475</v>
       </c>
       <c r="CP52" t="n">
-        <v>-0.529186686240193</v>
+        <v>-0.5291866862401938</v>
       </c>
       <c r="CQ52" t="n">
         <v>1</v>
@@ -56743,13 +56743,13 @@
         <v>17.817149360139</v>
       </c>
       <c r="GD52" t="n">
-        <v>195.8843408692714</v>
+        <v>195.8843408692713</v>
       </c>
       <c r="GE52" t="n">
         <v>-0.004492534230547332</v>
       </c>
       <c r="GF52" t="n">
-        <v>-0.273696361304601</v>
+        <v>-0.2736963613045997</v>
       </c>
       <c r="GG52" t="n">
         <v>1</v>
@@ -57399,13 +57399,13 @@
         <v>26.03315398430406</v>
       </c>
       <c r="AS53" t="n">
-        <v>-4.185361276933463</v>
+        <v>-4.185361276933236</v>
       </c>
       <c r="AT53" t="n">
         <v>-0.03802715592889141</v>
       </c>
       <c r="AU53" t="n">
-        <v>-0.07298338695894502</v>
+        <v>-0.07298338695894105</v>
       </c>
       <c r="AV53" t="n">
         <v>1</v>
@@ -57540,13 +57540,13 @@
         <v>19.24209327631613</v>
       </c>
       <c r="CN53" t="n">
-        <v>88.19775683135879</v>
+        <v>88.19775683135845</v>
       </c>
       <c r="CO53" t="n">
         <v>0.02773085948231207</v>
       </c>
       <c r="CP53" t="n">
-        <v>0.9995053298471932</v>
+        <v>0.999505329847193</v>
       </c>
       <c r="CQ53" t="n">
         <v>0</v>
@@ -57681,13 +57681,13 @@
         <v>22.58902988139615</v>
       </c>
       <c r="EI53" t="n">
-        <v>211.950518950205</v>
+        <v>211.9505189502051</v>
       </c>
       <c r="EJ53" t="n">
         <v>0.005792212006757475</v>
       </c>
       <c r="EK53" t="n">
-        <v>-0.529186686240193</v>
+        <v>-0.5291866862401938</v>
       </c>
       <c r="EL53" t="n">
         <v>1</v>
@@ -57822,13 +57822,13 @@
         <v>22.04708776193247</v>
       </c>
       <c r="GD53" t="n">
-        <v>-25.12804529840878</v>
+        <v>-25.12804529840957</v>
       </c>
       <c r="GE53" t="n">
         <v>-0.03156768979392504</v>
       </c>
       <c r="GF53" t="n">
-        <v>-0.4246426322585574</v>
+        <v>-0.4246426322585699</v>
       </c>
       <c r="GG53" t="n">
         <v>0</v>
@@ -58619,13 +58619,13 @@
         <v>26.03315398430406</v>
       </c>
       <c r="CN54" t="n">
-        <v>-4.185361276933463</v>
+        <v>-4.185361276933236</v>
       </c>
       <c r="CO54" t="n">
         <v>-0.03802715592889141</v>
       </c>
       <c r="CP54" t="n">
-        <v>-0.07298338695894502</v>
+        <v>-0.07298338695894105</v>
       </c>
       <c r="CQ54" t="n">
         <v>1</v>
@@ -58760,13 +58760,13 @@
         <v>19.24209327631613</v>
       </c>
       <c r="EI54" t="n">
-        <v>88.19775683135879</v>
+        <v>88.19775683135845</v>
       </c>
       <c r="EJ54" t="n">
         <v>0.02773085948231207</v>
       </c>
       <c r="EK54" t="n">
-        <v>0.9995053298471932</v>
+        <v>0.999505329847193</v>
       </c>
       <c r="EL54" t="n">
         <v>0</v>
@@ -59042,13 +59042,13 @@
         <v>17.817149360139</v>
       </c>
       <c r="HY54" t="n">
-        <v>195.8843408692714</v>
+        <v>195.8843408692713</v>
       </c>
       <c r="HZ54" t="n">
         <v>-0.004492534230547332</v>
       </c>
       <c r="IA54" t="n">
-        <v>-0.273696361304601</v>
+        <v>-0.2736963613045997</v>
       </c>
       <c r="IB54" t="n">
         <v>1</v>
@@ -59839,13 +59839,13 @@
         <v>26.03315398430406</v>
       </c>
       <c r="EI55" t="n">
-        <v>-4.185361276933463</v>
+        <v>-4.185361276933236</v>
       </c>
       <c r="EJ55" t="n">
         <v>-0.03802715592889141</v>
       </c>
       <c r="EK55" t="n">
-        <v>-0.07298338695894502</v>
+        <v>-0.07298338695894105</v>
       </c>
       <c r="EL55" t="n">
         <v>1</v>
@@ -59980,13 +59980,13 @@
         <v>22.58902988139615</v>
       </c>
       <c r="GD55" t="n">
-        <v>211.950518950205</v>
+        <v>211.9505189502051</v>
       </c>
       <c r="GE55" t="n">
         <v>0.005792212006757475</v>
       </c>
       <c r="GF55" t="n">
-        <v>-0.529186686240193</v>
+        <v>-0.5291866862401938</v>
       </c>
       <c r="GG55" t="n">
         <v>1</v>
@@ -60121,13 +60121,13 @@
         <v>22.04708776193247</v>
       </c>
       <c r="HY55" t="n">
-        <v>-25.12804529840878</v>
+        <v>-25.12804529840957</v>
       </c>
       <c r="HZ55" t="n">
         <v>-0.03156768979392504</v>
       </c>
       <c r="IA55" t="n">
-        <v>-0.4246426322585574</v>
+        <v>-0.4246426322585699</v>
       </c>
       <c r="IB55" t="n">
         <v>0</v>
@@ -61059,13 +61059,13 @@
         <v>19.24209327631613</v>
       </c>
       <c r="GD56" t="n">
-        <v>88.19775683135879</v>
+        <v>88.19775683135845</v>
       </c>
       <c r="GE56" t="n">
         <v>0.02773085948231207</v>
       </c>
       <c r="GF56" t="n">
-        <v>0.9995053298471932</v>
+        <v>0.999505329847193</v>
       </c>
       <c r="GG56" t="n">
         <v>0</v>
@@ -61341,13 +61341,13 @@
         <v>35.17717231077314</v>
       </c>
       <c r="JT56" t="n">
-        <v>-13.22557956059632</v>
+        <v>-13.22557956059597</v>
       </c>
       <c r="JU56" t="n">
         <v>0.008874889197968361</v>
       </c>
       <c r="JV56" t="n">
-        <v>-0.2287854992587356</v>
+        <v>-0.2287854992587298</v>
       </c>
       <c r="JW56" t="n">
         <v>0</v>
@@ -61715,13 +61715,13 @@
         <v>26.58950579654452</v>
       </c>
       <c r="AS57" t="n">
-        <v>109.8046324723726</v>
+        <v>109.8046324723727</v>
       </c>
       <c r="AT57" t="n">
         <v>0.0226264648257484</v>
       </c>
       <c r="AU57" t="n">
-        <v>0.9408533782760737</v>
+        <v>0.9408533782760736</v>
       </c>
       <c r="AV57" t="n">
         <v>0</v>
@@ -62138,13 +62138,13 @@
         <v>26.03315398430406</v>
       </c>
       <c r="GD57" t="n">
-        <v>-4.185361276933463</v>
+        <v>-4.185361276933236</v>
       </c>
       <c r="GE57" t="n">
         <v>-0.03802715592889141</v>
       </c>
       <c r="GF57" t="n">
-        <v>-0.07298338695894502</v>
+        <v>-0.07298338695894105</v>
       </c>
       <c r="GG57" t="n">
         <v>1</v>
@@ -62279,13 +62279,13 @@
         <v>22.58902988139615</v>
       </c>
       <c r="HY57" t="n">
-        <v>211.950518950205</v>
+        <v>211.9505189502051</v>
       </c>
       <c r="HZ57" t="n">
         <v>0.005792212006757475</v>
       </c>
       <c r="IA57" t="n">
-        <v>-0.529186686240193</v>
+        <v>-0.5291866862401938</v>
       </c>
       <c r="IB57" t="n">
         <v>1</v>
@@ -62800,7 +62800,7 @@
         <v>0.02407963300916956</v>
       </c>
       <c r="AU58" t="n">
-        <v>0.2538863043191921</v>
+        <v>0.2538863043191925</v>
       </c>
       <c r="AV58" t="n">
         <v>1</v>
@@ -62935,13 +62935,13 @@
         <v>26.58950579654452</v>
       </c>
       <c r="CN58" t="n">
-        <v>109.8046324723726</v>
+        <v>109.8046324723727</v>
       </c>
       <c r="CO58" t="n">
         <v>0.0226264648257484</v>
       </c>
       <c r="CP58" t="n">
-        <v>0.9408533782760737</v>
+        <v>0.9408533782760736</v>
       </c>
       <c r="CQ58" t="n">
         <v>0</v>
@@ -63358,13 +63358,13 @@
         <v>19.24209327631613</v>
       </c>
       <c r="HY58" t="n">
-        <v>88.19775683135879</v>
+        <v>88.19775683135845</v>
       </c>
       <c r="HZ58" t="n">
         <v>0.02773085948231207</v>
       </c>
       <c r="IA58" t="n">
-        <v>0.9995053298471932</v>
+        <v>0.999505329847193</v>
       </c>
       <c r="IB58" t="n">
         <v>0</v>
@@ -64020,7 +64020,7 @@
         <v>0.02407963300916956</v>
       </c>
       <c r="CP59" t="n">
-        <v>0.2538863043191921</v>
+        <v>0.2538863043191925</v>
       </c>
       <c r="CQ59" t="n">
         <v>1</v>
@@ -64155,13 +64155,13 @@
         <v>26.58950579654452</v>
       </c>
       <c r="EI59" t="n">
-        <v>109.8046324723726</v>
+        <v>109.8046324723727</v>
       </c>
       <c r="EJ59" t="n">
         <v>0.0226264648257484</v>
       </c>
       <c r="EK59" t="n">
-        <v>0.9408533782760737</v>
+        <v>0.9408533782760736</v>
       </c>
       <c r="EL59" t="n">
         <v>0</v>
@@ -64437,13 +64437,13 @@
         <v>26.03315398430406</v>
       </c>
       <c r="HY59" t="n">
-        <v>-4.185361276933463</v>
+        <v>-4.185361276933236</v>
       </c>
       <c r="HZ59" t="n">
         <v>-0.03802715592889141</v>
       </c>
       <c r="IA59" t="n">
-        <v>-0.07298338695894502</v>
+        <v>-0.07298338695894105</v>
       </c>
       <c r="IB59" t="n">
         <v>1</v>
@@ -65240,7 +65240,7 @@
         <v>0.02407963300916956</v>
       </c>
       <c r="EK60" t="n">
-        <v>0.2538863043191921</v>
+        <v>0.2538863043191925</v>
       </c>
       <c r="EL60" t="n">
         <v>1</v>
@@ -65657,13 +65657,13 @@
         <v>17.817149360139</v>
       </c>
       <c r="JT60" t="n">
-        <v>195.8843408692714</v>
+        <v>195.8843408692713</v>
       </c>
       <c r="JU60" t="n">
         <v>-0.004492534230547332</v>
       </c>
       <c r="JV60" t="n">
-        <v>-0.273696361304601</v>
+        <v>-0.2736963613045997</v>
       </c>
       <c r="JW60" t="n">
         <v>1</v>
@@ -66454,13 +66454,13 @@
         <v>26.58950579654452</v>
       </c>
       <c r="GD61" t="n">
-        <v>109.8046324723726</v>
+        <v>109.8046324723727</v>
       </c>
       <c r="GE61" t="n">
         <v>0.0226264648257484</v>
       </c>
       <c r="GF61" t="n">
-        <v>0.9408533782760737</v>
+        <v>0.9408533782760736</v>
       </c>
       <c r="GG61" t="n">
         <v>0</v>
@@ -66736,13 +66736,13 @@
         <v>22.04708776193247</v>
       </c>
       <c r="JT61" t="n">
-        <v>-25.12804529840878</v>
+        <v>-25.12804529840957</v>
       </c>
       <c r="JU61" t="n">
         <v>-0.03156768979392504</v>
       </c>
       <c r="JV61" t="n">
-        <v>-0.4246426322585574</v>
+        <v>-0.4246426322585699</v>
       </c>
       <c r="JW61" t="n">
         <v>0</v>
@@ -67110,13 +67110,13 @@
         <v>15.49632452935542</v>
       </c>
       <c r="AS62" t="n">
-        <v>221.8214035411778</v>
+        <v>221.8214035411777</v>
       </c>
       <c r="AT62" t="n">
         <v>0.02032127664973384</v>
       </c>
       <c r="AU62" t="n">
-        <v>-0.6668109054391327</v>
+        <v>-0.6668109054391318</v>
       </c>
       <c r="AV62" t="n">
         <v>0</v>
@@ -67539,7 +67539,7 @@
         <v>0.02407963300916956</v>
       </c>
       <c r="GF62" t="n">
-        <v>0.2538863043191921</v>
+        <v>0.2538863043191925</v>
       </c>
       <c r="GG62" t="n">
         <v>1</v>
@@ -68330,13 +68330,13 @@
         <v>15.49632452935542</v>
       </c>
       <c r="CN63" t="n">
-        <v>221.8214035411778</v>
+        <v>221.8214035411777</v>
       </c>
       <c r="CO63" t="n">
         <v>0.02032127664973384</v>
       </c>
       <c r="CP63" t="n">
-        <v>-0.6668109054391327</v>
+        <v>-0.6668109054391318</v>
       </c>
       <c r="CQ63" t="n">
         <v>0</v>
@@ -68753,13 +68753,13 @@
         <v>26.58950579654452</v>
       </c>
       <c r="HY63" t="n">
-        <v>109.8046324723726</v>
+        <v>109.8046324723727</v>
       </c>
       <c r="HZ63" t="n">
         <v>0.0226264648257484</v>
       </c>
       <c r="IA63" t="n">
-        <v>0.9408533782760737</v>
+        <v>0.9408533782760736</v>
       </c>
       <c r="IB63" t="n">
         <v>0</v>
@@ -68894,13 +68894,13 @@
         <v>22.58902988139615</v>
       </c>
       <c r="JT63" t="n">
-        <v>211.950518950205</v>
+        <v>211.9505189502051</v>
       </c>
       <c r="JU63" t="n">
         <v>0.005792212006757475</v>
       </c>
       <c r="JV63" t="n">
-        <v>-0.529186686240193</v>
+        <v>-0.5291866862401938</v>
       </c>
       <c r="JW63" t="n">
         <v>1</v>
@@ -69268,13 +69268,13 @@
         <v>23.34086993098518</v>
       </c>
       <c r="AS64" t="n">
-        <v>166.7177700084998</v>
+        <v>166.7177700084999</v>
       </c>
       <c r="AT64" t="n">
         <v>0.03732096483806242</v>
       </c>
       <c r="AU64" t="n">
-        <v>0.2297478994149678</v>
+        <v>0.2297478994149661</v>
       </c>
       <c r="AV64" t="n">
         <v>1</v>
@@ -69550,13 +69550,13 @@
         <v>15.49632452935542</v>
       </c>
       <c r="EI64" t="n">
-        <v>221.8214035411778</v>
+        <v>221.8214035411777</v>
       </c>
       <c r="EJ64" t="n">
         <v>0.02032127664973384</v>
       </c>
       <c r="EK64" t="n">
-        <v>-0.6668109054391327</v>
+        <v>-0.6668109054391318</v>
       </c>
       <c r="EL64" t="n">
         <v>0</v>
@@ -69838,7 +69838,7 @@
         <v>0.02407963300916956</v>
       </c>
       <c r="IA64" t="n">
-        <v>0.2538863043191921</v>
+        <v>0.2538863043191925</v>
       </c>
       <c r="IB64" t="n">
         <v>1</v>
@@ -69973,13 +69973,13 @@
         <v>19.24209327631613</v>
       </c>
       <c r="JT64" t="n">
-        <v>88.19775683135879</v>
+        <v>88.19775683135845</v>
       </c>
       <c r="JU64" t="n">
         <v>0.02773085948231207</v>
       </c>
       <c r="JV64" t="n">
-        <v>0.9995053298471932</v>
+        <v>0.999505329847193</v>
       </c>
       <c r="JW64" t="n">
         <v>0</v>

</xml_diff>